<commit_message>
Updated report and added multiple files and removed those not needed
</commit_message>
<xml_diff>
--- a/Burnout.xlsx
+++ b/Burnout.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Dropbox\Uni\CI301-IndividualProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Dropbox/Uni/CI301-IndividualProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="12360" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feature List Burndown 3 Oct 16" sheetId="1" r:id="rId1"/>
     <sheet name="Feature List Burndown 17 Oct" sheetId="4" r:id="rId2"/>
     <sheet name="Feature List Burndown 31 Oct" sheetId="5" r:id="rId3"/>
-    <sheet name="Project Feature List" sheetId="2" r:id="rId4"/>
-    <sheet name="DeliverablesTasks" sheetId="6" r:id="rId5"/>
+    <sheet name="Feature List Burndown 14 Nov" sheetId="7" r:id="rId4"/>
+    <sheet name="Project Feature List" sheetId="2" r:id="rId5"/>
+    <sheet name="DeliverablesTasks" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="86">
   <si>
     <t>Task</t>
   </si>
@@ -284,12 +284,18 @@
   </si>
   <si>
     <t>Iteration 2</t>
+  </si>
+  <si>
+    <t>14th Nov 2016 - 27th Nov 2016</t>
+  </si>
+  <si>
+    <t>Iteration 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -709,7 +715,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -832,6 +838,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1061,9 +1073,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1081,10 +1093,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13306959254568099"/>
-          <c:y val="1.8470685733562999E-2"/>
-          <c:w val="0.71469100453352397"/>
-          <c:h val="0.79831147760594201"/>
+          <c:x val="0.133069592545681"/>
+          <c:y val="0.018470685733563"/>
+          <c:w val="0.714691004533524"/>
+          <c:h val="0.798311477605942"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1153,37 +1165,37 @@
                   <c:v>22.95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.399999999999999</c:v>
+                  <c:v>20.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.849999999999998</c:v>
+                  <c:v>17.85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.299999999999997</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.749999999999996</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.199999999999996</c:v>
+                  <c:v>10.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.6499999999999959</c:v>
+                  <c:v>7.649999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0999999999999961</c:v>
+                  <c:v>5.099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5499999999999963</c:v>
+                  <c:v>2.549999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.5527136788005009E-15</c:v>
+                  <c:v>-3.5527136788005E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1C0B-4335-9EC1-2FE357BA21DD}"/>
             </c:ext>
@@ -1270,19 +1282,19 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1C0B-4335-9EC1-2FE357BA21DD}"/>
             </c:ext>
@@ -1297,11 +1309,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1959232256"/>
-        <c:axId val="-1989678864"/>
+        <c:axId val="-809978080"/>
+        <c:axId val="-808543520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1959232256"/>
+        <c:axId val="-809978080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,7 +1341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1989678864"/>
+        <c:crossAx val="-808543520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1337,7 +1349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989678864"/>
+        <c:axId val="-808543520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1959232256"/>
+        <c:crossAx val="-809978080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1388,16 +1400,16 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1415,10 +1427,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13306959254568099"/>
-          <c:y val="1.8470685733562999E-2"/>
-          <c:w val="0.71469100453352397"/>
-          <c:h val="0.79831147760594201"/>
+          <c:x val="0.133069592545681"/>
+          <c:y val="0.018470685733563"/>
+          <c:w val="0.714691004533524"/>
+          <c:h val="0.798311477605942"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1481,43 +1493,43 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7A87-40DB-A824-39E8CC826D42}"/>
             </c:ext>
@@ -1580,43 +1592,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7A87-40DB-A824-39E8CC826D42}"/>
             </c:ext>
@@ -1631,11 +1643,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1958679136"/>
-        <c:axId val="-1958671952"/>
+        <c:axId val="-808498080"/>
+        <c:axId val="-808490864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1958679136"/>
+        <c:axId val="-808498080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1663,7 +1675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1958671952"/>
+        <c:crossAx val="-808490864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1671,7 +1683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1958671952"/>
+        <c:axId val="-808490864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1700,7 +1712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1958679136"/>
+        <c:crossAx val="-808498080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1722,16 +1734,16 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1749,10 +1761,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13306959254568099"/>
-          <c:y val="1.8470685733562999E-2"/>
-          <c:w val="0.71469100453352397"/>
-          <c:h val="0.79831147760594201"/>
+          <c:x val="0.133069592545681"/>
+          <c:y val="0.018470685733563"/>
+          <c:w val="0.714691004533524"/>
+          <c:h val="0.798311477605942"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1824,34 +1836,34 @@
                   <c:v>24.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.349999999999998</c:v>
+                  <c:v>21.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.299999999999997</c:v>
+                  <c:v>18.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.249999999999996</c:v>
+                  <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.199999999999996</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.149999999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0999999999999952</c:v>
+                  <c:v>6.099999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0499999999999954</c:v>
+                  <c:v>3.049999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-4.4408920985006262E-15</c:v>
+                  <c:v>-4.44089209850063E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-151F-46E4-827B-3D3EDE01B3DC}"/>
             </c:ext>
@@ -1923,10 +1935,10 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>15.5</c:v>
@@ -1938,19 +1950,19 @@
                   <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.5</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-151F-46E4-827B-3D3EDE01B3DC}"/>
             </c:ext>
@@ -1965,11 +1977,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1958594928"/>
-        <c:axId val="-1958587744"/>
+        <c:axId val="-811638320"/>
+        <c:axId val="-811631136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1958594928"/>
+        <c:axId val="-811638320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,13 +2003,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1958587744"/>
+        <c:crossAx val="-811631136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2005,7 +2018,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1958587744"/>
+        <c:axId val="-811631136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,19 +2041,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1958594928"/>
+        <c:crossAx val="-811638320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2056,7 +2071,344 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.133069592545681"/>
+          <c:y val="0.018470685733563"/>
+          <c:w val="0.714691004533524"/>
+          <c:h val="0.798311477605942"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Feature List Burndown 14 Nov'!$F$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature List Burndown 14 Nov'!$F$17:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-151F-46E4-827B-3D3EDE01B3DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Feature List Burndown 14 Nov'!$F$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature List Burndown 14 Nov'!$F$18:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-151F-46E4-827B-3D3EDE01B3DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-748415472"/>
+        <c:axId val="-748408336"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-748415472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DAYS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-748408336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-748408336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>HOURS EFFORT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-748415472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2135,6 +2487,43 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>467784</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>245533</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2530,58 +2919,58 @@
       <selection activeCell="C25" sqref="C25:F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.5" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="5" customWidth="1"/>
     <col min="7" max="8" width="7.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="7.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="7" style="5" customWidth="1"/>
     <col min="13" max="13" width="7.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="7.625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="7.375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="7.625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="5.875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="51" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-    </row>
-    <row r="3" spans="2:17" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+    </row>
+    <row r="3" spans="2:17" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
@@ -2631,8 +3020,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="57" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -2682,8 +3071,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="58"/>
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2731,8 +3120,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="55" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="57" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -2782,8 +3171,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="57"/>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="59"/>
       <c r="C7" s="16" t="s">
         <v>3</v>
       </c>
@@ -2831,8 +3220,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="58"/>
       <c r="C8" s="16" t="s">
         <v>1</v>
       </c>
@@ -2880,8 +3269,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="55" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="57" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -2931,8 +3320,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
+    <row r="10" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="59"/>
       <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
@@ -2980,8 +3369,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
+    <row r="11" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="59"/>
       <c r="C11" s="16" t="s">
         <v>6</v>
       </c>
@@ -3029,8 +3418,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="56"/>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="58"/>
       <c r="C12" s="16" t="s">
         <v>7</v>
       </c>
@@ -3078,7 +3467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="24" t="s">
         <v>52</v>
       </c>
@@ -3129,8 +3518,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="55" t="s">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="57" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -3180,8 +3569,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="57"/>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="59"/>
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
@@ -3229,8 +3618,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="58"/>
       <c r="C16" s="16" t="s">
         <v>20</v>
       </c>
@@ -3278,13 +3667,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="54" t="s">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="23">
         <f>SUM(F4:F16)</f>
         <v>25.5</v>
@@ -3330,13 +3719,13 @@
         <v>-3.5527136788005009E-15</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="54" t="s">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B18" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="10">
         <f>SUM(F4:F16)</f>
         <v>25.5</v>
@@ -3388,7 +3777,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="25" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" ht="32" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>64</v>
       </c>
@@ -3423,58 +3812,58 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="3.5" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="5" customWidth="1"/>
     <col min="7" max="8" width="7.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="7.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="7" style="5" customWidth="1"/>
     <col min="13" max="13" width="7.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="7.625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="7.375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="7.625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="5.875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="51" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-    </row>
-    <row r="3" spans="2:17" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+    </row>
+    <row r="3" spans="2:17" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
@@ -3524,8 +3913,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="57" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -3575,8 +3964,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="58"/>
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -3624,8 +4013,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="55" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="57" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -3675,8 +4064,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="57"/>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="59"/>
       <c r="C7" s="16" t="s">
         <v>3</v>
       </c>
@@ -3724,8 +4113,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="58"/>
       <c r="C8" s="16" t="s">
         <v>1</v>
       </c>
@@ -3773,8 +4162,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="55" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="57" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -3824,8 +4213,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
+    <row r="10" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="59"/>
       <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
@@ -3873,8 +4262,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
+    <row r="11" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="59"/>
       <c r="C11" s="16" t="s">
         <v>6</v>
       </c>
@@ -3922,8 +4311,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="56"/>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="58"/>
       <c r="C12" s="16" t="s">
         <v>7</v>
       </c>
@@ -3971,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
         <v>52</v>
       </c>
@@ -4022,8 +4411,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="55" t="s">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="57" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -4073,8 +4462,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="57"/>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="59"/>
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
@@ -4122,8 +4511,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="58"/>
       <c r="C16" s="16" t="s">
         <v>20</v>
       </c>
@@ -4171,13 +4560,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="54" t="s">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="23">
         <f>SUM(F4:F16)</f>
         <v>25</v>
@@ -4223,13 +4612,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="54" t="s">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B18" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="10">
         <f>SUM(F4:F16)</f>
         <v>25</v>
@@ -4281,28 +4670,28 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="58" t="s">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B25" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="58"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="3" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="L2:P2"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4314,62 +4703,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="3.5" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="5" customWidth="1"/>
     <col min="7" max="8" width="7.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="7.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="7" style="5" customWidth="1"/>
     <col min="13" max="13" width="7.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="7.625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="7.375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="7.625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="5.875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="51" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-    </row>
-    <row r="3" spans="2:17" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+    </row>
+    <row r="3" spans="2:17" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
@@ -4419,8 +4808,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="57" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -4457,7 +4846,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="4">
         <v>0</v>
@@ -4467,11 +4856,11 @@
       </c>
       <c r="Q4" s="9">
         <f>SUM(G4:P4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="58"/>
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -4519,8 +4908,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="55" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="57" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -4560,18 +4949,18 @@
         <v>0</v>
       </c>
       <c r="O6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="4">
         <v>0</v>
       </c>
       <c r="Q6" s="9">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="57"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="59"/>
       <c r="C7" s="16" t="s">
         <v>3</v>
       </c>
@@ -4609,18 +4998,18 @@
         <v>0</v>
       </c>
       <c r="O7" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P7" s="4">
         <v>0</v>
       </c>
       <c r="Q7" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="58"/>
       <c r="C8" s="16" t="s">
         <v>1</v>
       </c>
@@ -4668,8 +5057,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="55" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="57" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -4709,18 +5098,18 @@
         <v>0</v>
       </c>
       <c r="O9" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P9" s="4">
         <v>0</v>
       </c>
       <c r="Q9" s="9">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="59"/>
       <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
@@ -4768,8 +5157,8 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
+    <row r="11" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="59"/>
       <c r="C11" s="16" t="s">
         <v>6</v>
       </c>
@@ -4817,8 +5206,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="56"/>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="58"/>
       <c r="C12" s="16" t="s">
         <v>7</v>
       </c>
@@ -4866,7 +5255,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
         <v>52</v>
       </c>
@@ -4907,18 +5296,18 @@
         <v>0</v>
       </c>
       <c r="O13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P13" s="4">
         <v>0</v>
       </c>
       <c r="Q13" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="57" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -4966,8 +5355,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="57"/>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="59"/>
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
@@ -5015,8 +5404,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="58"/>
       <c r="C16" s="16" t="s">
         <v>20</v>
       </c>
@@ -5064,13 +5453,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="54" t="s">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="23">
         <f>SUM(F4:F16)</f>
         <v>30.5</v>
@@ -5116,13 +5505,13 @@
         <v>-4.4408920985006262E-15</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="54" t="s">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B18" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="10">
         <f>SUM(F4:F16)</f>
         <v>30.5</v>
@@ -5157,15 +5546,15 @@
       </c>
       <c r="N18" s="6">
         <f t="shared" si="2"/>
-        <v>15.5</v>
+        <v>14.5</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="2"/>
-        <v>15.5</v>
+        <v>10.5</v>
       </c>
       <c r="P18" s="7">
         <f t="shared" si="2"/>
-        <v>15.5</v>
+        <v>10.5</v>
       </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="2"/>
@@ -5176,16 +5565,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5195,23 +5584,908 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:V18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="52" customWidth="1"/>
+    <col min="7" max="8" width="7.5" style="52" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="52" customWidth="1"/>
+    <col min="10" max="10" width="7.5" style="52" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="52" customWidth="1"/>
+    <col min="12" max="12" width="7" style="52" customWidth="1"/>
+    <col min="13" max="13" width="7.5" style="52" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="52" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="52" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="52" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" style="52" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+    </row>
+    <row r="3" spans="2:17" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="9">
+        <f>SUM(G4:P4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="58"/>
+      <c r="C5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" ref="Q5:Q16" si="0">SUM(G5:P5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="17">
+        <v>2.1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="59"/>
+      <c r="C7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="58"/>
+      <c r="C8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="59"/>
+      <c r="C10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="17">
+        <v>3.2</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="59"/>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="58"/>
+      <c r="C12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="17">
+        <v>3.4</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="17">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="59"/>
+      <c r="C15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="17">
+        <v>5.2</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="58"/>
+      <c r="C16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="17">
+        <v>5.3</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="23">
+        <f>SUM(F4:F16)</f>
+        <v>1.5</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" ref="G17:P17" si="1">F17-$F$17/10</f>
+        <v>1.35</v>
+      </c>
+      <c r="H17" s="18">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="1"/>
+        <v>1.0500000000000003</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" si="1"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="K17" s="19">
+        <f t="shared" si="1"/>
+        <v>0.75000000000000022</v>
+      </c>
+      <c r="L17" s="18">
+        <f t="shared" si="1"/>
+        <v>0.6000000000000002</v>
+      </c>
+      <c r="M17" s="18">
+        <f t="shared" si="1"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="N17" s="18">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000016</v>
+      </c>
+      <c r="O17" s="18">
+        <f t="shared" si="1"/>
+        <v>0.15000000000000016</v>
+      </c>
+      <c r="P17" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B18" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="10">
+        <f>SUM(F4:F16)</f>
+        <v>1.5</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" ref="G18:P18" si="2">F18-(SUM(G4:G16))</f>
+        <v>1.5</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="22">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="P18" s="7">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B8"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="5" customWidth="1"/>
-    <col min="3" max="3" width="113.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5955,7 +7229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -5963,13 +7237,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="109.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>36</v>
       </c>
@@ -5977,11 +7251,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="29"/>
     </row>
-    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>1</v>
       </c>
@@ -5989,7 +7263,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>2</v>
       </c>
@@ -5997,7 +7271,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>3</v>
       </c>
@@ -6005,7 +7279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>4</v>
       </c>
@@ -6013,7 +7287,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>5</v>
       </c>
@@ -6021,7 +7295,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>6</v>
       </c>
@@ -6029,7 +7303,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>7</v>
       </c>
@@ -6037,7 +7311,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>8</v>
       </c>
@@ -6045,7 +7319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>9</v>
       </c>
@@ -6053,7 +7327,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>10</v>
       </c>
@@ -6061,7 +7335,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>11</v>
       </c>
@@ -6069,7 +7343,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>12</v>
       </c>
@@ -6077,7 +7351,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>13</v>
       </c>
@@ -6085,7 +7359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <v>14</v>
       </c>
@@ -6093,7 +7367,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>15</v>
       </c>

</xml_diff>